<commit_message>
Início relatório - Experimento 4
</commit_message>
<xml_diff>
--- a/Exp4/Dados/Buck/2.xlsx
+++ b/Exp4/Dados/Buck/2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>D</t>
   </si>
@@ -45,22 +45,19 @@
     <t>Vr</t>
   </si>
   <si>
-    <t>1.02</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>0.62</t>
+    <t>Ia</t>
+  </si>
+  <si>
+    <t>R:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,10 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,15 +401,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F3" sqref="F3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,8 +422,17 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1">
+        <v>5.3</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20</v>
       </c>
@@ -436,7 +443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
@@ -446,11 +453,15 @@
       <c r="C3">
         <v>102</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
+      <c r="E3">
+        <v>0.62</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3/$I$1</f>
+        <v>0.1169811320754717</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40</v>
       </c>
@@ -460,11 +471,15 @@
       <c r="C4">
         <v>234</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
+      <c r="E4">
+        <v>0.76</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F6" si="0">E4/$I$1</f>
+        <v>0.14339622641509434</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
@@ -474,11 +489,15 @@
       <c r="C5">
         <v>390</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
+      <c r="E5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.169811320754717</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>60</v>
       </c>
@@ -488,8 +507,12 @@
       <c r="C6">
         <v>574</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
+      <c r="E6">
+        <v>1.02</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.19245283018867926</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adicionando dados (torque) ao relatório
</commit_message>
<xml_diff>
--- a/Exp4/Dados/Buck/2.xlsx
+++ b/Exp4/Dados/Buck/2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>D</t>
   </si>
@@ -27,18 +27,6 @@
     <t>w</t>
   </si>
   <si>
-    <t>4.32</t>
-  </si>
-  <si>
-    <t>5.4</t>
-  </si>
-  <si>
-    <t>3.08</t>
-  </si>
-  <si>
-    <t>2.18</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -48,7 +36,10 @@
     <t>Ia</t>
   </si>
   <si>
-    <t>R:</t>
+    <t>Rr</t>
+  </si>
+  <si>
+    <t>Tm</t>
   </si>
 </sst>
 </file>
@@ -56,7 +47,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -95,11 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,15 +393,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,35 +412,42 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1">
         <v>5.3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="H2" t="e">
+        <f>B2*F2</f>
+        <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+      <c r="B3" s="2">
+        <v>2.1800000000000002</v>
       </c>
       <c r="C3">
         <v>102</v>
@@ -457,16 +456,20 @@
         <v>0.62</v>
       </c>
       <c r="F3" s="3">
-        <f>E3/$I$1</f>
+        <f>E3/$M$1</f>
         <v>0.1169811320754717</v>
       </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H6" si="0">B3*F3</f>
+        <v>0.25501886792452833</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4">
+        <v>3.08</v>
       </c>
       <c r="C4">
         <v>234</v>
@@ -475,16 +478,20 @@
         <v>0.76</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F6" si="0">E4/$I$1</f>
+        <f>E4/$M$1</f>
         <v>0.14339622641509434</v>
       </c>
+      <c r="H4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.44166037735849056</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
+      <c r="B5">
+        <v>4.32</v>
       </c>
       <c r="C5">
         <v>390</v>
@@ -493,16 +500,20 @@
         <v>0.9</v>
       </c>
       <c r="F5" s="3">
+        <f>E5/$M$1</f>
+        <v>0.169811320754717</v>
+      </c>
+      <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>0.169811320754717</v>
+        <v>0.73358490566037748</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>60</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
+      <c r="B6">
+        <v>5.4</v>
       </c>
       <c r="C6">
         <v>574</v>
@@ -511,8 +522,12 @@
         <v>1.02</v>
       </c>
       <c r="F6" s="3">
+        <f>E6/$M$1</f>
+        <v>0.19245283018867926</v>
+      </c>
+      <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>0.19245283018867926</v>
+        <v>1.0392452830188681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>